<commit_message>
clean up faq excel
</commit_message>
<xml_diff>
--- a/faq.xlsx
+++ b/faq.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="47">
   <si>
     <t xml:space="preserve">CASE_ID</t>
   </si>
@@ -31,13 +31,22 @@
     <t xml:space="preserve">INTENT_LIST</t>
   </si>
   <si>
+    <t xml:space="preserve">EXPRESSION_CASE</t>
+  </si>
+  <si>
     <t xml:space="preserve">JUMP_TO_CASE</t>
   </si>
   <si>
     <t xml:space="preserve">RESPONSE_ID_LIST</t>
   </si>
   <si>
-    <t xml:space="preserve">SET_CONTEXT_EXPRESION</t>
+    <t xml:space="preserve">ACTION_BUTTON_ID_LIST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PROCEDURE_ADVISORY_ID_LIST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SET_CONTEXT_EXPRESSION</t>
   </si>
   <si>
     <t xml:space="preserve">1_START</t>
@@ -52,13 +61,19 @@
     <t xml:space="preserve">LEAF11</t>
   </si>
   <si>
+    <t xml:space="preserve">RESPONSE_002</t>
+  </si>
+  <si>
     <t xml:space="preserve">3_LEAF_11</t>
   </si>
   <si>
+    <t xml:space="preserve">RESPONSE_003</t>
+  </si>
+  <si>
     <t xml:space="preserve">2A_NODE_12</t>
   </si>
   <si>
-    <t xml:space="preserve">RESPONSE_002</t>
+    <t xml:space="preserve">RESPONSE_004</t>
   </si>
   <si>
     <t xml:space="preserve">2B_NODE_121</t>
@@ -67,25 +82,40 @@
     <t xml:space="preserve">LEAF121</t>
   </si>
   <si>
+    <t xml:space="preserve">RESPONSE_005</t>
+  </si>
+  <si>
     <t xml:space="preserve">2B_NODE_122</t>
   </si>
   <si>
+    <t xml:space="preserve">RESPONSE_006</t>
+  </si>
+  <si>
     <t xml:space="preserve">2B_NODE_123</t>
   </si>
   <si>
     <t xml:space="preserve">LEAF123</t>
   </si>
   <si>
+    <t xml:space="preserve">RESPONSE_007</t>
+  </si>
+  <si>
     <t xml:space="preserve">3_LEAF_121</t>
   </si>
   <si>
+    <t xml:space="preserve">RESPONSE_008</t>
+  </si>
+  <si>
     <t xml:space="preserve">3_LEAF_123</t>
   </si>
   <si>
+    <t xml:space="preserve">RESPONSE_009</t>
+  </si>
+  <si>
     <t xml:space="preserve">2A_NODE_13</t>
   </si>
   <si>
-    <t xml:space="preserve">RESPONSE_003</t>
+    <t xml:space="preserve">RESPONSE_010</t>
   </si>
   <si>
     <t xml:space="preserve">2B_NODE_131</t>
@@ -94,95 +124,43 @@
     <t xml:space="preserve">LEAF131</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">2B_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">NODE_132</t>
-    </r>
+    <t xml:space="preserve">RESPONSE_011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2B_NODE_132</t>
   </si>
   <si>
     <t xml:space="preserve">LEAF132</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">2B_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">NODE_133</t>
-    </r>
+    <t xml:space="preserve">RESPONSE_012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2B_NODE_133</t>
   </si>
   <si>
     <t xml:space="preserve">LEAF133</t>
   </si>
   <si>
+    <t xml:space="preserve">RESPONSE_013</t>
+  </si>
+  <si>
     <t xml:space="preserve">3_LEAF_131</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">3_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">LEAF_132</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">2B_NODE_132</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">3_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">LEAF_133</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">2B_NODE_133</t>
+    <t xml:space="preserve">RESPONSE_014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3_LEAF_132</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESPONSE_015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3_LEAF_133</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESPONSE_016</t>
   </si>
 </sst>
 </file>
@@ -192,7 +170,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -213,11 +191,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -267,7 +240,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -288,20 +261,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
+      <selection pane="topLeft" activeCell="H15" activeCellId="0" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="25.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="24.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="30.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="28.12"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -323,160 +299,211 @@
       <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>7</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="0" t="s">
         <v>9</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>12</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>9</v>
+        <v>16</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>17</v>
+      <c r="E8" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>13</v>
+      <c r="F9" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>21</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" s="1"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>23</v>
+        <v>30</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>25</v>
+        <v>30</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>27</v>
+        <v>30</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>22</v>
+        <v>32</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>30</v>
+        <v>35</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>32</v>
+        <v>38</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test data and test script, only exceptions and a few are not yet under coverage
</commit_message>
<xml_diff>
--- a/faq.xlsx
+++ b/faq.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="48">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -91,6 +91,9 @@
     <t xml:space="preserve">RESPONSE_001</t>
   </si>
   <si>
+    <t xml:space="preserve">BUTTON_11, BUTTON_12, BUTTON_13</t>
+  </si>
+  <si>
     <t xml:space="preserve">3_LEAF_11, 2_NODE_12, 2_NODE_13</t>
   </si>
   <si>
@@ -100,12 +103,18 @@
     <t xml:space="preserve">RESPONSE_002</t>
   </si>
   <si>
+    <t xml:space="preserve">CAROUSEL_1, CAROUSEL_2, CAROUSEL_3</t>
+  </si>
+  <si>
     <t xml:space="preserve">2_NODE_12</t>
   </si>
   <si>
     <t xml:space="preserve">RESPONSE_003</t>
   </si>
   <si>
+    <t xml:space="preserve">BUTTON_121, BUTTON_123, BUTTON_132</t>
+  </si>
+  <si>
     <t xml:space="preserve">3_LEAF_121, 3_LEAF_123, 3_LEAF_132</t>
   </si>
   <si>
@@ -127,6 +136,9 @@
     <t xml:space="preserve">RESPONSE_006</t>
   </si>
   <si>
+    <t xml:space="preserve">BUTTON_131, BUTTON_132, BUTTON_133, BUTTON_123</t>
+  </si>
+  <si>
     <t xml:space="preserve">3_LEAF_131, 3_LEAF_132, 3_LEAF_133, 3_LEAF_123</t>
   </si>
   <si>
@@ -145,7 +157,13 @@
     <t xml:space="preserve">3_LEAF_133</t>
   </si>
   <si>
+    <t xml:space="preserve">3_JUMP_TO_1</t>
+  </si>
+  <si>
     <t xml:space="preserve">RESPONSE_009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESPONSE_010</t>
   </si>
 </sst>
 </file>
@@ -155,7 +173,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -176,6 +194,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -220,12 +243,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -248,11 +275,11 @@
   </sheetPr>
   <dimension ref="A1:T11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="13.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.98"/>
@@ -260,7 +287,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="24.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="30.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="21.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="21.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="21.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="27.63"/>
@@ -345,9 +372,11 @@
       <c r="F2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="1"/>
+      <c r="G2" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="I2" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -355,10 +384,13 @@
         <v>20</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -366,14 +398,16 @@
         <v>20</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" s="1"/>
+        <v>29</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="I4" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -381,10 +415,10 @@
         <v>20</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -392,10 +426,10 @@
         <v>20</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -403,14 +437,16 @@
         <v>20</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G7" s="1"/>
+        <v>37</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="I7" s="0" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -418,10 +454,10 @@
         <v>20</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -429,11 +465,11 @@
         <v>20</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -441,14 +477,28 @@
         <v>20</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="1"/>
+      <c r="B11" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>47</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
changing sample test case to reflect optional respond ID list
</commit_message>
<xml_diff>
--- a/faq.xlsx
+++ b/faq.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="47">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -119,9 +119,6 @@
   </si>
   <si>
     <t xml:space="preserve">3_LEAF_121</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RESPONSE_004</t>
   </si>
   <si>
     <t xml:space="preserve">3_LEAF_123</t>
@@ -173,7 +170,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -194,11 +191,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -243,16 +235,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -275,11 +263,11 @@
   </sheetPr>
   <dimension ref="A1:T11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="13.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.98"/>
@@ -417,19 +405,17 @@
       <c r="C5" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>33</v>
-      </c>
+      <c r="F5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
         <v>20</v>
       </c>
       <c r="C6" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -437,16 +423,16 @@
         <v>20</v>
       </c>
       <c r="C7" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="I7" s="0" t="s">
         <v>38</v>
-      </c>
-      <c r="I7" s="0" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -454,10 +440,10 @@
         <v>20</v>
       </c>
       <c r="C8" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -465,11 +451,11 @@
         <v>20</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -477,13 +463,13 @@
         <v>20</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="F10" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -491,13 +477,13 @@
         <v>20</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E11" s="0" t="s">
         <v>21</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>